<commit_message>
Story 8 - modelos
</commit_message>
<xml_diff>
--- a/Docs/Project/taskboard.xlsx
+++ b/Docs/Project/taskboard.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/dfb9b990915f6edd/MIT IA/git/mit_ds_course/Docs/Project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="8_{70B88BAA-752F-456B-938A-4F6D20DE3B6C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{2DD09D5C-DE7B-4F5E-956D-6645FCE1B33B}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="8_{70B88BAA-752F-456B-938A-4F6D20DE3B6C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{3FD0F816-4A0F-4128-AD84-9BE33698ED65}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{EFC1725C-2304-4691-9531-9BACDA3C9584}"/>
   </bookViews>
@@ -621,7 +621,7 @@
   <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="52.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -856,7 +856,7 @@
         <v>3</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>11</v>
+        <v>52</v>
       </c>
       <c r="G9" s="2" t="s">
         <v>37</v>

</xml_diff>